<commit_message>
Updated code and report backup
</commit_message>
<xml_diff>
--- a/TestHarness/Results/Results.xlsx
+++ b/TestHarness/Results/Results.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ciaran\Workspace\MscDissertation\TestHarness\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC220075-B619-413B-A2A0-DAA73C2AE629}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FDEBC8-B405-4D08-BE3F-CAE7952E1C5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{4D699BBE-F084-483C-BBD6-55F837A4A712}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4D699BBE-F084-483C-BBD6-55F837A4A712}"/>
   </bookViews>
   <sheets>
     <sheet name="EASOM_FINAL" sheetId="2" r:id="rId1"/>
     <sheet name="BEALE_FINAL" sheetId="3" r:id="rId2"/>
     <sheet name="BOOTHS_FUNCTION_FINAL" sheetId="4" r:id="rId3"/>
     <sheet name="Summary" sheetId="1" r:id="rId4"/>
-    <sheet name="Config" sheetId="5" r:id="rId5"/>
+    <sheet name="Config" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">BEALE_FINAL!$A$1:$H$215</definedName>
@@ -111,19 +111,7 @@
     <t>Particle Number</t>
   </si>
   <si>
-    <t>Centalised - 2</t>
-  </si>
-  <si>
     <t>BOOTHS_FUNCTION_FINAL</t>
-  </si>
-  <si>
-    <t>Distributed - 2</t>
-  </si>
-  <si>
-    <t>Centalised - 4</t>
-  </si>
-  <si>
-    <t>Distributed - 4</t>
   </si>
   <si>
     <t>BEALE_FINAL</t>
@@ -132,16 +120,28 @@
     <t>EASOM_FINAL</t>
   </si>
   <si>
-    <t>Centalised - 8</t>
+    <t>Centalised TTS - 2</t>
   </si>
   <si>
-    <t>Distributed - 8</t>
+    <t>Distributed TTS - 2</t>
   </si>
   <si>
-    <t>Centalised - 10</t>
+    <t>Centalised TTS - 4</t>
   </si>
   <si>
-    <t>Distributed - 10</t>
+    <t>Distributed TTS - 4</t>
+  </si>
+  <si>
+    <t>Centalised TTS - 8</t>
+  </si>
+  <si>
+    <t>Distributed TTS - 8</t>
+  </si>
+  <si>
+    <t>Centalised TTS - 10</t>
+  </si>
+  <si>
+    <t>Distributed TTS - 10</t>
   </si>
 </sst>
 </file>
@@ -289,7 +289,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Centalised - 2</c:v>
+                  <c:v>Centalised TTS - 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -364,34 +364,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4205</c:v>
+                  <c:v>2364</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8828</c:v>
+                  <c:v>4578</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14003</c:v>
+                  <c:v>6681</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19742</c:v>
+                  <c:v>9776</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27418</c:v>
+                  <c:v>12875</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39291</c:v>
+                  <c:v>19400</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>52039</c:v>
+                  <c:v>24188</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60327</c:v>
+                  <c:v>28344</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>78404</c:v>
+                  <c:v>36510</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>112258</c:v>
+                  <c:v>50887</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -412,7 +412,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Distributed - 2</c:v>
+                  <c:v>Distributed TTS - 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -487,34 +487,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>5291</c:v>
+                  <c:v>3551</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7370</c:v>
+                  <c:v>2545</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13213</c:v>
+                  <c:v>7217</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18240</c:v>
+                  <c:v>9145</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23625</c:v>
+                  <c:v>12404</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29258</c:v>
+                  <c:v>14614</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35314</c:v>
+                  <c:v>17662</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40600</c:v>
+                  <c:v>20410</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>49349</c:v>
+                  <c:v>24803</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>56502</c:v>
+                  <c:v>29327</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -535,7 +535,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Centalised - 4</c:v>
+                  <c:v>Centalised TTS - 4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -610,34 +610,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3842</c:v>
+                  <c:v>2297</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8676</c:v>
+                  <c:v>4449</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13934</c:v>
+                  <c:v>6731</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19301</c:v>
+                  <c:v>9779</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27981</c:v>
+                  <c:v>13835</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40426</c:v>
+                  <c:v>18945</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>51825</c:v>
+                  <c:v>23920</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>61134</c:v>
+                  <c:v>27520</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>81726</c:v>
+                  <c:v>38057</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>119800</c:v>
+                  <c:v>51263</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -658,7 +658,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Distributed - 4</c:v>
+                  <c:v>Distributed TTS - 4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -733,34 +733,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>5630</c:v>
+                  <c:v>3287</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10308</c:v>
+                  <c:v>5154</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13959</c:v>
+                  <c:v>7583</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19389</c:v>
+                  <c:v>7434</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24069</c:v>
+                  <c:v>11663</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27959</c:v>
+                  <c:v>14158</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33992</c:v>
+                  <c:v>16690</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>39246</c:v>
+                  <c:v>19008</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45128</c:v>
+                  <c:v>21444</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>48906</c:v>
+                  <c:v>23923</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -781,7 +781,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Centalised - 8</c:v>
+                  <c:v>Centalised TTS - 8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -856,34 +856,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4775</c:v>
+                  <c:v>2313</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9276</c:v>
+                  <c:v>4313</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14489</c:v>
+                  <c:v>6694</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20336</c:v>
+                  <c:v>9749</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27615</c:v>
+                  <c:v>13176</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40594</c:v>
+                  <c:v>18825</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>49939</c:v>
+                  <c:v>23905</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>65653</c:v>
+                  <c:v>30373</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>79632</c:v>
+                  <c:v>36939</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>112751</c:v>
+                  <c:v>52918</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -904,7 +904,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Distributed - 8</c:v>
+                  <c:v>Distributed TTS - 8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -979,34 +979,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>7153</c:v>
+                  <c:v>3925</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10988</c:v>
+                  <c:v>6217</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15164</c:v>
+                  <c:v>8228</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20080</c:v>
+                  <c:v>9961</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24213</c:v>
+                  <c:v>12298</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28980</c:v>
+                  <c:v>14661</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33915</c:v>
+                  <c:v>17383</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>39852</c:v>
+                  <c:v>14769</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44175</c:v>
+                  <c:v>22707</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>49696</c:v>
+                  <c:v>24623</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1027,7 +1027,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Centalised - 10</c:v>
+                  <c:v>Centalised TTS - 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1108,34 +1108,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4417</c:v>
+                  <c:v>2388</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9294</c:v>
+                  <c:v>4783</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14964</c:v>
+                  <c:v>8033</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22167</c:v>
+                  <c:v>11264</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>33411</c:v>
+                  <c:v>16012</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45841</c:v>
+                  <c:v>21732</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56124</c:v>
+                  <c:v>27103</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70674</c:v>
+                  <c:v>33907</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>98879</c:v>
+                  <c:v>47329</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>160899</c:v>
+                  <c:v>78160</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1156,7 +1156,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Distributed - 10</c:v>
+                  <c:v>Distributed TTS - 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1237,34 +1237,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>7860</c:v>
+                  <c:v>4385</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10223</c:v>
+                  <c:v>5449</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16299</c:v>
+                  <c:v>8556</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20567</c:v>
+                  <c:v>11039</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25084</c:v>
+                  <c:v>13091</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29629</c:v>
+                  <c:v>15548</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33713</c:v>
+                  <c:v>17736</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>39174</c:v>
+                  <c:v>20474</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44859</c:v>
+                  <c:v>22619</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51248</c:v>
+                  <c:v>26300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2027,15 +2027,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1019175</xdr:colOff>
+      <xdr:colOff>723899</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2464,7 +2464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{139960D8-BF09-417C-B87C-EC077B5A6850}">
   <dimension ref="A1:H215"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -13700,7 +13700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2CE85EA-18B2-45A4-9309-731D29A15ED9}">
   <dimension ref="A1:H215"/>
   <sheetViews>
-    <sheetView topLeftCell="A179" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B206" sqref="B206"/>
     </sheetView>
   </sheetViews>
@@ -19318,22 +19318,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6321EF05-1508-47EE-9B24-FEEFC230091E}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -19341,7 +19341,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -19349,16 +19349,16 @@
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>17</v>
@@ -19379,35 +19379,35 @@
       </c>
       <c r="C5" s="3" cm="1">
         <f t="array" aca="1" ref="C5" ca="1">INDIRECT(B1&amp;"!D34")</f>
-        <v>4205</v>
+        <v>2364</v>
       </c>
       <c r="D5" s="3" cm="1">
         <f t="array" aca="1" ref="D5" ca="1">INDIRECT(B1&amp;"!G34")</f>
-        <v>5291</v>
+        <v>3551</v>
       </c>
       <c r="E5" s="1" cm="1">
         <f t="array" aca="1" ref="E5" ca="1">INDIRECT(B1&amp;"!D78")</f>
-        <v>3842</v>
+        <v>2297</v>
       </c>
       <c r="F5" s="1" cm="1">
         <f t="array" aca="1" ref="F5" ca="1">INDIRECT(B1&amp;"!G78")</f>
-        <v>5630</v>
+        <v>3287</v>
       </c>
       <c r="G5" s="1" cm="1">
         <f t="array" aca="1" ref="G5" ca="1">INDIRECT(B1&amp;"!D161")</f>
-        <v>4775</v>
+        <v>2313</v>
       </c>
       <c r="H5" s="1" cm="1">
         <f t="array" aca="1" ref="H5" ca="1">INDIRECT(B1&amp;"!G161")</f>
-        <v>7153</v>
+        <v>3925</v>
       </c>
       <c r="I5" s="1" cm="1">
         <f t="array" aca="1" ref="I5" ca="1">INDIRECT(B1&amp;"!D206")</f>
-        <v>4417</v>
+        <v>2388</v>
       </c>
       <c r="J5" s="1" cm="1">
         <f t="array" aca="1" ref="J5" ca="1">INDIRECT(B1&amp;"!G206")</f>
-        <v>7860</v>
+        <v>4385</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -19417,35 +19417,35 @@
       </c>
       <c r="C6" s="1" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">INDIRECT(B1&amp;"!D39")</f>
-        <v>8828</v>
+        <v>4578</v>
       </c>
       <c r="D6" s="1" cm="1">
         <f t="array" aca="1" ref="D6" ca="1">INDIRECT(B1&amp;"!G39")</f>
-        <v>7370</v>
+        <v>2545</v>
       </c>
       <c r="E6" s="1" cm="1">
         <f t="array" aca="1" ref="E6" ca="1">INDIRECT(B1&amp;"!D81")</f>
-        <v>8676</v>
+        <v>4449</v>
       </c>
       <c r="F6" s="1" cm="1">
         <f t="array" aca="1" ref="F6" ca="1">INDIRECT(B1&amp;"!G81")</f>
-        <v>10308</v>
+        <v>5154</v>
       </c>
       <c r="G6" s="1" cm="1">
         <f t="array" aca="1" ref="G6" ca="1">INDIRECT(B1&amp;"!D163")</f>
-        <v>9276</v>
+        <v>4313</v>
       </c>
       <c r="H6" s="1" cm="1">
         <f t="array" aca="1" ref="H6" ca="1">INDIRECT(B1&amp;"!G163")</f>
-        <v>10988</v>
+        <v>6217</v>
       </c>
       <c r="I6" s="1" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">INDIRECT(B1&amp;"!D207")</f>
-        <v>9294</v>
+        <v>4783</v>
       </c>
       <c r="J6" s="1" cm="1">
         <f t="array" aca="1" ref="J6" ca="1">INDIRECT(B1&amp;"!G207")</f>
-        <v>10223</v>
+        <v>5449</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -19455,35 +19455,35 @@
       </c>
       <c r="C7" s="1" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">INDIRECT(B1&amp;"!D40")</f>
-        <v>14003</v>
+        <v>6681</v>
       </c>
       <c r="D7" s="1" cm="1">
         <f t="array" aca="1" ref="D7" ca="1">INDIRECT(B1&amp;"!G40")</f>
-        <v>13213</v>
+        <v>7217</v>
       </c>
       <c r="E7" s="1" cm="1">
         <f t="array" aca="1" ref="E7" ca="1">INDIRECT(B1&amp;"!D84")</f>
-        <v>13934</v>
+        <v>6731</v>
       </c>
       <c r="F7" s="1" cm="1">
         <f t="array" aca="1" ref="F7" ca="1">INDIRECT(B1&amp;"!G84")</f>
-        <v>13959</v>
+        <v>7583</v>
       </c>
       <c r="G7" s="1" cm="1">
         <f t="array" aca="1" ref="G7" ca="1">INDIRECT(B1&amp;"!D165")</f>
-        <v>14489</v>
+        <v>6694</v>
       </c>
       <c r="H7" s="1" cm="1">
         <f t="array" aca="1" ref="H7" ca="1">INDIRECT(B1&amp;"!G165")</f>
-        <v>15164</v>
+        <v>8228</v>
       </c>
       <c r="I7" s="1" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">INDIRECT(B1&amp;"!D208")</f>
-        <v>14964</v>
+        <v>8033</v>
       </c>
       <c r="J7" s="1" cm="1">
         <f t="array" aca="1" ref="J7" ca="1">INDIRECT(B1&amp;"!G208")</f>
-        <v>16299</v>
+        <v>8556</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -19493,35 +19493,35 @@
       </c>
       <c r="C8" s="1" cm="1">
         <f t="array" aca="1" ref="C8" ca="1">INDIRECT(B1&amp;"!D41")</f>
-        <v>19742</v>
+        <v>9776</v>
       </c>
       <c r="D8" s="1" cm="1">
         <f t="array" aca="1" ref="D8" ca="1">INDIRECT(B1&amp;"!G41")</f>
-        <v>18240</v>
+        <v>9145</v>
       </c>
       <c r="E8" s="1" cm="1">
         <f t="array" aca="1" ref="E8" ca="1">INDIRECT(B1&amp;"!D87")</f>
-        <v>19301</v>
+        <v>9779</v>
       </c>
       <c r="F8" s="1" cm="1">
         <f t="array" aca="1" ref="F8" ca="1">INDIRECT(B1&amp;"!G87")</f>
-        <v>19389</v>
+        <v>7434</v>
       </c>
       <c r="G8" s="1" cm="1">
         <f t="array" aca="1" ref="G8" ca="1">INDIRECT(B1&amp;"!D167")</f>
-        <v>20336</v>
+        <v>9749</v>
       </c>
       <c r="H8" s="1" cm="1">
         <f t="array" aca="1" ref="H8" ca="1">INDIRECT(B1&amp;"!G167")</f>
-        <v>20080</v>
+        <v>9961</v>
       </c>
       <c r="I8" s="1" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">INDIRECT(B1&amp;"!D209")</f>
-        <v>22167</v>
+        <v>11264</v>
       </c>
       <c r="J8" s="1" cm="1">
         <f t="array" aca="1" ref="J8" ca="1">INDIRECT(B1&amp;"!G209")</f>
-        <v>20567</v>
+        <v>11039</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -19531,35 +19531,35 @@
       </c>
       <c r="C9" s="1" cm="1">
         <f t="array" aca="1" ref="C9" ca="1">INDIRECT(B1&amp;"!D42")</f>
-        <v>27418</v>
+        <v>12875</v>
       </c>
       <c r="D9" s="1" cm="1">
         <f t="array" aca="1" ref="D9" ca="1">INDIRECT(B1&amp;"!G42")</f>
-        <v>23625</v>
+        <v>12404</v>
       </c>
       <c r="E9" s="1" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">INDIRECT(B1&amp;"!D88")</f>
-        <v>27981</v>
+        <v>13835</v>
       </c>
       <c r="F9" s="1" cm="1">
         <f t="array" aca="1" ref="F9" ca="1">INDIRECT(B1&amp;"!G88")</f>
-        <v>24069</v>
+        <v>11663</v>
       </c>
       <c r="G9" s="1" cm="1">
         <f t="array" aca="1" ref="G9" ca="1">INDIRECT(B1&amp;"!D169")</f>
-        <v>27615</v>
+        <v>13176</v>
       </c>
       <c r="H9" s="1" cm="1">
         <f t="array" aca="1" ref="H9" ca="1">INDIRECT(B1&amp;"!G169")</f>
-        <v>24213</v>
+        <v>12298</v>
       </c>
       <c r="I9" s="1" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">INDIRECT(B1&amp;"!D210")</f>
-        <v>33411</v>
+        <v>16012</v>
       </c>
       <c r="J9" s="1" cm="1">
         <f t="array" aca="1" ref="J9" ca="1">INDIRECT(B1&amp;"!G210")</f>
-        <v>25084</v>
+        <v>13091</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -19569,35 +19569,35 @@
       </c>
       <c r="C10" s="1" cm="1">
         <f t="array" aca="1" ref="C10" ca="1">INDIRECT(B1&amp;"!D43")</f>
-        <v>39291</v>
+        <v>19400</v>
       </c>
       <c r="D10" s="1" cm="1">
         <f t="array" aca="1" ref="D10" ca="1">INDIRECT(B1&amp;"!G43")</f>
-        <v>29258</v>
+        <v>14614</v>
       </c>
       <c r="E10" s="1" cm="1">
         <f t="array" aca="1" ref="E10" ca="1">INDIRECT(B1&amp;"!D89")</f>
-        <v>40426</v>
+        <v>18945</v>
       </c>
       <c r="F10" s="1" cm="1">
         <f t="array" aca="1" ref="F10" ca="1">INDIRECT(B1&amp;"!G89")</f>
-        <v>27959</v>
+        <v>14158</v>
       </c>
       <c r="G10" s="1" cm="1">
         <f t="array" aca="1" ref="G10" ca="1">INDIRECT(B1&amp;"!D171")</f>
-        <v>40594</v>
+        <v>18825</v>
       </c>
       <c r="H10" s="1" cm="1">
         <f t="array" aca="1" ref="H10" ca="1">INDIRECT(B1&amp;"!G171")</f>
-        <v>28980</v>
+        <v>14661</v>
       </c>
       <c r="I10" s="1" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">INDIRECT(B1&amp;"!D211")</f>
-        <v>45841</v>
+        <v>21732</v>
       </c>
       <c r="J10" s="1" cm="1">
         <f t="array" aca="1" ref="J10" ca="1">INDIRECT(B1&amp;"!G211")</f>
-        <v>29629</v>
+        <v>15548</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -19607,35 +19607,35 @@
       </c>
       <c r="C11" s="1" cm="1">
         <f t="array" aca="1" ref="C11" ca="1">INDIRECT(B1&amp;"!D44")</f>
-        <v>52039</v>
+        <v>24188</v>
       </c>
       <c r="D11" s="1" cm="1">
         <f t="array" aca="1" ref="D11" ca="1">INDIRECT(B1&amp;"!G44")</f>
-        <v>35314</v>
+        <v>17662</v>
       </c>
       <c r="E11" s="1" cm="1">
         <f t="array" aca="1" ref="E11" ca="1">INDIRECT(B1&amp;"!D90")</f>
-        <v>51825</v>
+        <v>23920</v>
       </c>
       <c r="F11" s="1" cm="1">
         <f t="array" aca="1" ref="F11" ca="1">INDIRECT(B1&amp;"!G90")</f>
-        <v>33992</v>
+        <v>16690</v>
       </c>
       <c r="G11" s="1" cm="1">
         <f t="array" aca="1" ref="G11" ca="1">INDIRECT(B1&amp;"!D173")</f>
-        <v>49939</v>
+        <v>23905</v>
       </c>
       <c r="H11" s="1" cm="1">
         <f t="array" aca="1" ref="H11" ca="1">INDIRECT(B1&amp;"!G173")</f>
-        <v>33915</v>
+        <v>17383</v>
       </c>
       <c r="I11" s="1" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">INDIRECT(B1&amp;"!D212")</f>
-        <v>56124</v>
+        <v>27103</v>
       </c>
       <c r="J11" s="1" cm="1">
         <f t="array" aca="1" ref="J11" ca="1">INDIRECT(B1&amp;"!G212")</f>
-        <v>33713</v>
+        <v>17736</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -19645,35 +19645,35 @@
       </c>
       <c r="C12" s="1" cm="1">
         <f t="array" aca="1" ref="C12" ca="1">INDIRECT(B1&amp;"!D45")</f>
-        <v>60327</v>
+        <v>28344</v>
       </c>
       <c r="D12" s="1" cm="1">
         <f t="array" aca="1" ref="D12" ca="1">INDIRECT(B1&amp;"!G45")</f>
-        <v>40600</v>
+        <v>20410</v>
       </c>
       <c r="E12" s="1" cm="1">
         <f t="array" aca="1" ref="E12" ca="1">INDIRECT(B1&amp;"!D91")</f>
-        <v>61134</v>
+        <v>27520</v>
       </c>
       <c r="F12" s="1" cm="1">
         <f t="array" aca="1" ref="F12" ca="1">INDIRECT(B1&amp;"!G91")</f>
-        <v>39246</v>
+        <v>19008</v>
       </c>
       <c r="G12" s="1" cm="1">
         <f t="array" aca="1" ref="G12" ca="1">INDIRECT(B1&amp;"!D175")</f>
-        <v>65653</v>
+        <v>30373</v>
       </c>
       <c r="H12" s="1" cm="1">
         <f t="array" aca="1" ref="H12" ca="1">INDIRECT(B1&amp;"!G175")</f>
-        <v>39852</v>
+        <v>14769</v>
       </c>
       <c r="I12" s="1" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">INDIRECT(B1&amp;"!D213")</f>
-        <v>70674</v>
+        <v>33907</v>
       </c>
       <c r="J12" s="1" cm="1">
         <f t="array" aca="1" ref="J12" ca="1">INDIRECT(B1&amp;"!G213")</f>
-        <v>39174</v>
+        <v>20474</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -19683,35 +19683,35 @@
       </c>
       <c r="C13" s="1" cm="1">
         <f t="array" aca="1" ref="C13" ca="1">INDIRECT(B1&amp;"!D46")</f>
-        <v>78404</v>
+        <v>36510</v>
       </c>
       <c r="D13" s="1" cm="1">
         <f t="array" aca="1" ref="D13" ca="1">INDIRECT(B1&amp;"!G46")</f>
-        <v>49349</v>
+        <v>24803</v>
       </c>
       <c r="E13" s="1" cm="1">
         <f t="array" aca="1" ref="E13" ca="1">INDIRECT(B1&amp;"!D92")</f>
-        <v>81726</v>
+        <v>38057</v>
       </c>
       <c r="F13" s="1" cm="1">
         <f t="array" aca="1" ref="F13" ca="1">INDIRECT(B1&amp;"!G92")</f>
-        <v>45128</v>
+        <v>21444</v>
       </c>
       <c r="G13" s="1" cm="1">
         <f t="array" aca="1" ref="G13" ca="1">INDIRECT(B1&amp;"!D176")</f>
-        <v>79632</v>
+        <v>36939</v>
       </c>
       <c r="H13" s="1" cm="1">
         <f t="array" aca="1" ref="H13" ca="1">INDIRECT(B1&amp;"!G176")</f>
-        <v>44175</v>
+        <v>22707</v>
       </c>
       <c r="I13" s="1" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">INDIRECT(B1&amp;"!D214")</f>
-        <v>98879</v>
+        <v>47329</v>
       </c>
       <c r="J13" s="1" cm="1">
         <f t="array" aca="1" ref="J13" ca="1">INDIRECT(B1&amp;"!G214")</f>
-        <v>44859</v>
+        <v>22619</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -19721,35 +19721,35 @@
       </c>
       <c r="C14" s="1" cm="1">
         <f t="array" aca="1" ref="C14" ca="1">INDIRECT(B1&amp;"!D47")</f>
-        <v>112258</v>
+        <v>50887</v>
       </c>
       <c r="D14" s="1" cm="1">
         <f t="array" aca="1" ref="D14" ca="1">INDIRECT(B1&amp;"!G47")</f>
-        <v>56502</v>
+        <v>29327</v>
       </c>
       <c r="E14" s="1" cm="1">
         <f t="array" aca="1" ref="E14" ca="1">INDIRECT(B1&amp;"!D93")</f>
-        <v>119800</v>
+        <v>51263</v>
       </c>
       <c r="F14" s="1" cm="1">
         <f t="array" aca="1" ref="F14" ca="1">INDIRECT(B1&amp;"!G93")</f>
-        <v>48906</v>
+        <v>23923</v>
       </c>
       <c r="G14" s="1" cm="1">
         <f t="array" aca="1" ref="G14" ca="1">INDIRECT(B1&amp;"!D177")</f>
-        <v>112751</v>
+        <v>52918</v>
       </c>
       <c r="H14" s="1" cm="1">
         <f t="array" aca="1" ref="H14" ca="1">INDIRECT(B1&amp;"!G177")</f>
-        <v>49696</v>
+        <v>24623</v>
       </c>
       <c r="I14" s="1" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">INDIRECT(B1&amp;"!D215")</f>
-        <v>160899</v>
+        <v>78160</v>
       </c>
       <c r="J14" s="1" cm="1">
         <f t="array" aca="1" ref="J14" ca="1">INDIRECT(B1&amp;"!G215")</f>
-        <v>51248</v>
+        <v>26300</v>
       </c>
     </row>
   </sheetData>
@@ -19785,17 +19785,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with first draft. Wohoo!!
</commit_message>
<xml_diff>
--- a/TestHarness/Results/Results.xlsx
+++ b/TestHarness/Results/Results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ciaran\Workspace\MscDissertation\TestHarness\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E23E49-49E1-4C7A-8FF7-C262FD12E516}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A94A8D7-A75C-4D2A-9259-CD8627B1D809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{4D699BBE-F084-483C-BBD6-55F837A4A712}"/>
   </bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="52">
   <si>
     <t>SWARM_NUMBER</t>
   </si>
@@ -202,18 +202,6 @@
   </si>
   <si>
     <t>Average</t>
-  </si>
-  <si>
-    <t>Average Cent</t>
-  </si>
-  <si>
-    <t>Average Distributed</t>
-  </si>
-  <si>
-    <t>Distributed</t>
-  </si>
-  <si>
-    <t>Centralised</t>
   </si>
   <si>
     <t>Beale</t>
@@ -416,7 +404,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -429,6 +416,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
@@ -553,34 +541,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2364</c:v>
+                  <c:v>4205</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4578</c:v>
+                  <c:v>8828</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6681</c:v>
+                  <c:v>14003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9776</c:v>
+                  <c:v>19742</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12875</c:v>
+                  <c:v>27418</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19400</c:v>
+                  <c:v>39291</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24188</c:v>
+                  <c:v>52039</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28344</c:v>
+                  <c:v>60327</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36510</c:v>
+                  <c:v>78404</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50887</c:v>
+                  <c:v>112258</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -676,34 +664,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3551</c:v>
+                  <c:v>5291</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2545</c:v>
+                  <c:v>7370</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7217</c:v>
+                  <c:v>13213</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9145</c:v>
+                  <c:v>18240</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12404</c:v>
+                  <c:v>23625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14614</c:v>
+                  <c:v>29258</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17662</c:v>
+                  <c:v>35314</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20410</c:v>
+                  <c:v>40600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24803</c:v>
+                  <c:v>49349</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29327</c:v>
+                  <c:v>56502</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -799,34 +787,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2297</c:v>
+                  <c:v>3842</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4449</c:v>
+                  <c:v>8676</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6731</c:v>
+                  <c:v>13934</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9779</c:v>
+                  <c:v>19301</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13835</c:v>
+                  <c:v>27981</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18945</c:v>
+                  <c:v>40426</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23920</c:v>
+                  <c:v>51825</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27520</c:v>
+                  <c:v>61134</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>38057</c:v>
+                  <c:v>81726</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51263</c:v>
+                  <c:v>119800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -922,34 +910,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3287</c:v>
+                  <c:v>5630</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5154</c:v>
+                  <c:v>10308</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7583</c:v>
+                  <c:v>13959</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7434</c:v>
+                  <c:v>19389</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11663</c:v>
+                  <c:v>24069</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14158</c:v>
+                  <c:v>27959</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16690</c:v>
+                  <c:v>33992</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19008</c:v>
+                  <c:v>39246</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21444</c:v>
+                  <c:v>45128</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>23923</c:v>
+                  <c:v>48906</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1045,34 +1033,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2313</c:v>
+                  <c:v>4775</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4313</c:v>
+                  <c:v>9276</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6694</c:v>
+                  <c:v>14489</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9749</c:v>
+                  <c:v>20336</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13176</c:v>
+                  <c:v>27615</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18825</c:v>
+                  <c:v>40594</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23905</c:v>
+                  <c:v>49939</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30373</c:v>
+                  <c:v>65653</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36939</c:v>
+                  <c:v>79632</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52918</c:v>
+                  <c:v>112751</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1168,34 +1156,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3925</c:v>
+                  <c:v>7153</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6217</c:v>
+                  <c:v>10988</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8228</c:v>
+                  <c:v>15164</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9961</c:v>
+                  <c:v>20080</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12298</c:v>
+                  <c:v>24213</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14661</c:v>
+                  <c:v>28980</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17383</c:v>
+                  <c:v>33915</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14769</c:v>
+                  <c:v>39852</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22707</c:v>
+                  <c:v>44175</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>24623</c:v>
+                  <c:v>49696</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1297,34 +1285,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2388</c:v>
+                  <c:v>4417</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4783</c:v>
+                  <c:v>9294</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8033</c:v>
+                  <c:v>14964</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11264</c:v>
+                  <c:v>22167</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16012</c:v>
+                  <c:v>33411</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21732</c:v>
+                  <c:v>45841</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27103</c:v>
+                  <c:v>56124</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33907</c:v>
+                  <c:v>70674</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47329</c:v>
+                  <c:v>98879</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>78160</c:v>
+                  <c:v>160899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1426,34 +1414,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4385</c:v>
+                  <c:v>7860</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5449</c:v>
+                  <c:v>10223</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8556</c:v>
+                  <c:v>16299</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11039</c:v>
+                  <c:v>20567</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13091</c:v>
+                  <c:v>25084</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15548</c:v>
+                  <c:v>29629</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17736</c:v>
+                  <c:v>33713</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20474</c:v>
+                  <c:v>39174</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22619</c:v>
+                  <c:v>44859</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>26300</c:v>
+                  <c:v>51248</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1772,34 +1760,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>63</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>54</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>54</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>52</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>51</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1895,34 +1883,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>56</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>55</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>54</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>54</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>54</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2018,34 +2006,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>58</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>52</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>53</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2141,34 +2129,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>59</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>51</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>51</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2264,34 +2252,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>61</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>54</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>52</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>53</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2387,34 +2375,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>61</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>61</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>52</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>49</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>53</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2516,34 +2504,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>62</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>54</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>52</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>52</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2645,34 +2633,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>55</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>56</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>55</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>52</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2992,34 +2980,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2364</c:v>
+                  <c:v>4205</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4578</c:v>
+                  <c:v>8828</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6681</c:v>
+                  <c:v>14003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9776</c:v>
+                  <c:v>19742</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12875</c:v>
+                  <c:v>27418</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19400</c:v>
+                  <c:v>39291</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24188</c:v>
+                  <c:v>52039</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>28344</c:v>
+                  <c:v>60327</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36510</c:v>
+                  <c:v>78404</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50887</c:v>
+                  <c:v>112258</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3115,34 +3103,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2297</c:v>
+                  <c:v>3842</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4449</c:v>
+                  <c:v>8676</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6731</c:v>
+                  <c:v>13934</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9779</c:v>
+                  <c:v>19301</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13835</c:v>
+                  <c:v>27981</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18945</c:v>
+                  <c:v>40426</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23920</c:v>
+                  <c:v>51825</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27520</c:v>
+                  <c:v>61134</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>38057</c:v>
+                  <c:v>81726</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51263</c:v>
+                  <c:v>119800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3238,34 +3226,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2313</c:v>
+                  <c:v>4775</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4313</c:v>
+                  <c:v>9276</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6694</c:v>
+                  <c:v>14489</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9749</c:v>
+                  <c:v>20336</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13176</c:v>
+                  <c:v>27615</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18825</c:v>
+                  <c:v>40594</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23905</c:v>
+                  <c:v>49939</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30373</c:v>
+                  <c:v>65653</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36939</c:v>
+                  <c:v>79632</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52918</c:v>
+                  <c:v>112751</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3361,34 +3349,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2388</c:v>
+                  <c:v>4417</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4783</c:v>
+                  <c:v>9294</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8033</c:v>
+                  <c:v>14964</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11264</c:v>
+                  <c:v>22167</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16012</c:v>
+                  <c:v>33411</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21732</c:v>
+                  <c:v>45841</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27103</c:v>
+                  <c:v>56124</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33907</c:v>
+                  <c:v>70674</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47329</c:v>
+                  <c:v>98879</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>78160</c:v>
+                  <c:v>160899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3829,34 +3817,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>63</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>54</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>54</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>52</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>51</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3952,34 +3940,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>58</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>52</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>53</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>51</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4075,34 +4063,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>61</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>54</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>52</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>53</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4198,34 +4186,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>62</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>54</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>52</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>52</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4663,34 +4651,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3551</c:v>
+                  <c:v>5291</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2545</c:v>
+                  <c:v>7370</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7217</c:v>
+                  <c:v>13213</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9145</c:v>
+                  <c:v>18240</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12404</c:v>
+                  <c:v>23625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14614</c:v>
+                  <c:v>29258</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17662</c:v>
+                  <c:v>35314</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20410</c:v>
+                  <c:v>40600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24803</c:v>
+                  <c:v>49349</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29327</c:v>
+                  <c:v>56502</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4786,34 +4774,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3287</c:v>
+                  <c:v>5630</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5154</c:v>
+                  <c:v>10308</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7583</c:v>
+                  <c:v>13959</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7434</c:v>
+                  <c:v>19389</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11663</c:v>
+                  <c:v>24069</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14158</c:v>
+                  <c:v>27959</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16690</c:v>
+                  <c:v>33992</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19008</c:v>
+                  <c:v>39246</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21444</c:v>
+                  <c:v>45128</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>23923</c:v>
+                  <c:v>48906</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4909,34 +4897,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3925</c:v>
+                  <c:v>7153</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6217</c:v>
+                  <c:v>10988</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8228</c:v>
+                  <c:v>15164</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9961</c:v>
+                  <c:v>20080</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12298</c:v>
+                  <c:v>24213</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14661</c:v>
+                  <c:v>28980</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17383</c:v>
+                  <c:v>33915</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14769</c:v>
+                  <c:v>39852</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22707</c:v>
+                  <c:v>44175</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>24623</c:v>
+                  <c:v>49696</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5032,34 +5020,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4385</c:v>
+                  <c:v>7860</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5449</c:v>
+                  <c:v>10223</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8556</c:v>
+                  <c:v>16299</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11039</c:v>
+                  <c:v>20567</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13091</c:v>
+                  <c:v>25084</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15548</c:v>
+                  <c:v>29629</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17736</c:v>
+                  <c:v>33713</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20474</c:v>
+                  <c:v>39174</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22619</c:v>
+                  <c:v>44859</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>26300</c:v>
+                  <c:v>51248</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5500,34 +5488,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>56</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>55</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>54</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>54</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>54</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5623,34 +5611,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>59</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>51</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>51</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5746,34 +5734,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>61</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>61</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>52</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>49</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>53</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5869,34 +5857,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>55</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>56</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>55</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>52</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -26987,8 +26975,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L80" sqref="L80"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4:V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27016,7 +27004,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -27092,73 +27080,73 @@
       </c>
       <c r="C5" s="3" cm="1">
         <f t="array" aca="1" ref="C5" ca="1">INDIRECT(B1&amp;"!D34")</f>
-        <v>2364</v>
+        <v>4205</v>
       </c>
       <c r="D5" s="3" cm="1">
         <f t="array" aca="1" ref="D5" ca="1">INDIRECT(B1&amp;"!G34")</f>
-        <v>3551</v>
+        <v>5291</v>
       </c>
       <c r="E5" s="1" cm="1">
         <f t="array" aca="1" ref="E5" ca="1">INDIRECT(B1&amp;"!D78")</f>
-        <v>2297</v>
+        <v>3842</v>
       </c>
       <c r="F5" s="1" cm="1">
         <f t="array" aca="1" ref="F5" ca="1">INDIRECT(B1&amp;"!G78")</f>
-        <v>3287</v>
+        <v>5630</v>
       </c>
       <c r="G5" s="1" cm="1">
         <f t="array" aca="1" ref="G5" ca="1">INDIRECT(B1&amp;"!D161")</f>
-        <v>2313</v>
+        <v>4775</v>
       </c>
       <c r="H5" s="1" cm="1">
         <f t="array" aca="1" ref="H5" ca="1">INDIRECT(B1&amp;"!G161")</f>
-        <v>3925</v>
+        <v>7153</v>
       </c>
       <c r="I5" s="1" cm="1">
         <f t="array" aca="1" ref="I5" ca="1">INDIRECT(B1&amp;"!D206")</f>
-        <v>2388</v>
+        <v>4417</v>
       </c>
       <c r="J5" s="1" cm="1">
         <f t="array" aca="1" ref="J5" ca="1">INDIRECT(B1&amp;"!G206")</f>
-        <v>4385</v>
+        <v>7860</v>
       </c>
       <c r="L5" s="1">
         <v>100000</v>
       </c>
       <c r="M5" s="1" cm="1">
         <f t="array" aca="1" ref="M5:M14" ca="1">C5:C14</f>
-        <v>2364</v>
+        <v>4205</v>
       </c>
       <c r="N5" s="1" cm="1">
         <f t="array" aca="1" ref="N5:N14" ca="1">E5:E14</f>
-        <v>2297</v>
+        <v>3842</v>
       </c>
       <c r="O5" s="1" cm="1">
         <f t="array" aca="1" ref="O5:O14" ca="1">G5:G14</f>
-        <v>2313</v>
+        <v>4775</v>
       </c>
       <c r="P5" s="1" cm="1">
         <f t="array" aca="1" ref="P5:P14" ca="1">I5:I14</f>
-        <v>2388</v>
+        <v>4417</v>
       </c>
       <c r="R5" s="1">
         <v>100000</v>
       </c>
       <c r="S5" s="1" cm="1">
         <f t="array" aca="1" ref="S5:S14" ca="1">D5:D14</f>
-        <v>3551</v>
+        <v>5291</v>
       </c>
       <c r="T5" s="1" cm="1">
         <f t="array" aca="1" ref="T5:T14" ca="1">F5:F14</f>
-        <v>3287</v>
+        <v>5630</v>
       </c>
       <c r="U5" s="1" cm="1">
         <f t="array" aca="1" ref="U5:U14" ca="1">H5:H14</f>
-        <v>3925</v>
+        <v>7153</v>
       </c>
       <c r="V5" s="1" cm="1">
         <f t="array" aca="1" ref="V5:V14" ca="1">J5:J14</f>
-        <v>4385</v>
+        <v>7860</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -27168,35 +27156,35 @@
       </c>
       <c r="C6" s="1" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">INDIRECT(B1&amp;"!D39")</f>
-        <v>4578</v>
+        <v>8828</v>
       </c>
       <c r="D6" s="1" cm="1">
         <f t="array" aca="1" ref="D6" ca="1">INDIRECT(B1&amp;"!G39")</f>
-        <v>2545</v>
+        <v>7370</v>
       </c>
       <c r="E6" s="1" cm="1">
         <f t="array" aca="1" ref="E6" ca="1">INDIRECT(B1&amp;"!D81")</f>
-        <v>4449</v>
+        <v>8676</v>
       </c>
       <c r="F6" s="1" cm="1">
         <f t="array" aca="1" ref="F6" ca="1">INDIRECT(B1&amp;"!G81")</f>
-        <v>5154</v>
+        <v>10308</v>
       </c>
       <c r="G6" s="1" cm="1">
         <f t="array" aca="1" ref="G6" ca="1">INDIRECT(B1&amp;"!D163")</f>
-        <v>4313</v>
+        <v>9276</v>
       </c>
       <c r="H6" s="1" cm="1">
         <f t="array" aca="1" ref="H6" ca="1">INDIRECT(B1&amp;"!G163")</f>
-        <v>6217</v>
+        <v>10988</v>
       </c>
       <c r="I6" s="1" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">INDIRECT(B1&amp;"!D207")</f>
-        <v>4783</v>
+        <v>9294</v>
       </c>
       <c r="J6" s="1" cm="1">
         <f t="array" aca="1" ref="J6" ca="1">INDIRECT(B1&amp;"!G207")</f>
-        <v>5449</v>
+        <v>10223</v>
       </c>
       <c r="L6" s="1">
         <f>L5 + 100000</f>
@@ -27204,19 +27192,19 @@
       </c>
       <c r="M6" s="1">
         <f ca="1"/>
-        <v>4578</v>
+        <v>8828</v>
       </c>
       <c r="N6" s="1">
         <f ca="1"/>
-        <v>4449</v>
+        <v>8676</v>
       </c>
       <c r="O6" s="1">
         <f ca="1"/>
-        <v>4313</v>
+        <v>9276</v>
       </c>
       <c r="P6" s="1">
         <f ca="1"/>
-        <v>4783</v>
+        <v>9294</v>
       </c>
       <c r="R6" s="1">
         <f>R5 + 100000</f>
@@ -27224,19 +27212,19 @@
       </c>
       <c r="S6" s="1">
         <f ca="1"/>
-        <v>2545</v>
+        <v>7370</v>
       </c>
       <c r="T6" s="1">
         <f ca="1"/>
-        <v>5154</v>
+        <v>10308</v>
       </c>
       <c r="U6" s="1">
         <f ca="1"/>
-        <v>6217</v>
+        <v>10988</v>
       </c>
       <c r="V6" s="1">
         <f ca="1"/>
-        <v>5449</v>
+        <v>10223</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -27246,35 +27234,35 @@
       </c>
       <c r="C7" s="1" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">INDIRECT(B1&amp;"!D40")</f>
-        <v>6681</v>
+        <v>14003</v>
       </c>
       <c r="D7" s="1" cm="1">
         <f t="array" aca="1" ref="D7" ca="1">INDIRECT(B1&amp;"!G40")</f>
-        <v>7217</v>
+        <v>13213</v>
       </c>
       <c r="E7" s="1" cm="1">
         <f t="array" aca="1" ref="E7" ca="1">INDIRECT(B1&amp;"!D84")</f>
-        <v>6731</v>
+        <v>13934</v>
       </c>
       <c r="F7" s="1" cm="1">
         <f t="array" aca="1" ref="F7" ca="1">INDIRECT(B1&amp;"!G84")</f>
-        <v>7583</v>
+        <v>13959</v>
       </c>
       <c r="G7" s="1" cm="1">
         <f t="array" aca="1" ref="G7" ca="1">INDIRECT(B1&amp;"!D165")</f>
-        <v>6694</v>
+        <v>14489</v>
       </c>
       <c r="H7" s="1" cm="1">
         <f t="array" aca="1" ref="H7" ca="1">INDIRECT(B1&amp;"!G165")</f>
-        <v>8228</v>
+        <v>15164</v>
       </c>
       <c r="I7" s="1" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">INDIRECT(B1&amp;"!D208")</f>
-        <v>8033</v>
+        <v>14964</v>
       </c>
       <c r="J7" s="1" cm="1">
         <f t="array" aca="1" ref="J7" ca="1">INDIRECT(B1&amp;"!G208")</f>
-        <v>8556</v>
+        <v>16299</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" ref="L7:L14" si="1">L6 + 100000</f>
@@ -27282,19 +27270,19 @@
       </c>
       <c r="M7" s="1">
         <f ca="1"/>
-        <v>6681</v>
+        <v>14003</v>
       </c>
       <c r="N7" s="1">
         <f ca="1"/>
-        <v>6731</v>
+        <v>13934</v>
       </c>
       <c r="O7" s="1">
         <f ca="1"/>
-        <v>6694</v>
+        <v>14489</v>
       </c>
       <c r="P7" s="1">
         <f ca="1"/>
-        <v>8033</v>
+        <v>14964</v>
       </c>
       <c r="R7" s="1">
         <f t="shared" ref="R7:R14" si="2">R6 + 100000</f>
@@ -27302,19 +27290,19 @@
       </c>
       <c r="S7" s="1">
         <f ca="1"/>
-        <v>7217</v>
+        <v>13213</v>
       </c>
       <c r="T7" s="1">
         <f ca="1"/>
-        <v>7583</v>
+        <v>13959</v>
       </c>
       <c r="U7" s="1">
         <f ca="1"/>
-        <v>8228</v>
+        <v>15164</v>
       </c>
       <c r="V7" s="1">
         <f ca="1"/>
-        <v>8556</v>
+        <v>16299</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -27324,35 +27312,35 @@
       </c>
       <c r="C8" s="1" cm="1">
         <f t="array" aca="1" ref="C8" ca="1">INDIRECT(B1&amp;"!D41")</f>
-        <v>9776</v>
+        <v>19742</v>
       </c>
       <c r="D8" s="1" cm="1">
         <f t="array" aca="1" ref="D8" ca="1">INDIRECT(B1&amp;"!G41")</f>
-        <v>9145</v>
+        <v>18240</v>
       </c>
       <c r="E8" s="1" cm="1">
         <f t="array" aca="1" ref="E8" ca="1">INDIRECT(B1&amp;"!D87")</f>
-        <v>9779</v>
+        <v>19301</v>
       </c>
       <c r="F8" s="1" cm="1">
         <f t="array" aca="1" ref="F8" ca="1">INDIRECT(B1&amp;"!G87")</f>
-        <v>7434</v>
+        <v>19389</v>
       </c>
       <c r="G8" s="1" cm="1">
         <f t="array" aca="1" ref="G8" ca="1">INDIRECT(B1&amp;"!D167")</f>
-        <v>9749</v>
+        <v>20336</v>
       </c>
       <c r="H8" s="1" cm="1">
         <f t="array" aca="1" ref="H8" ca="1">INDIRECT(B1&amp;"!G167")</f>
-        <v>9961</v>
+        <v>20080</v>
       </c>
       <c r="I8" s="1" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">INDIRECT(B1&amp;"!D209")</f>
-        <v>11264</v>
+        <v>22167</v>
       </c>
       <c r="J8" s="1" cm="1">
         <f t="array" aca="1" ref="J8" ca="1">INDIRECT(B1&amp;"!G209")</f>
-        <v>11039</v>
+        <v>20567</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="1"/>
@@ -27360,19 +27348,19 @@
       </c>
       <c r="M8" s="1">
         <f ca="1"/>
-        <v>9776</v>
+        <v>19742</v>
       </c>
       <c r="N8" s="1">
         <f ca="1"/>
-        <v>9779</v>
+        <v>19301</v>
       </c>
       <c r="O8" s="1">
         <f ca="1"/>
-        <v>9749</v>
+        <v>20336</v>
       </c>
       <c r="P8" s="1">
         <f ca="1"/>
-        <v>11264</v>
+        <v>22167</v>
       </c>
       <c r="R8" s="1">
         <f t="shared" si="2"/>
@@ -27380,19 +27368,19 @@
       </c>
       <c r="S8" s="1">
         <f ca="1"/>
-        <v>9145</v>
+        <v>18240</v>
       </c>
       <c r="T8" s="1">
         <f ca="1"/>
-        <v>7434</v>
+        <v>19389</v>
       </c>
       <c r="U8" s="1">
         <f ca="1"/>
-        <v>9961</v>
+        <v>20080</v>
       </c>
       <c r="V8" s="1">
         <f ca="1"/>
-        <v>11039</v>
+        <v>20567</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -27402,35 +27390,35 @@
       </c>
       <c r="C9" s="1" cm="1">
         <f t="array" aca="1" ref="C9" ca="1">INDIRECT(B1&amp;"!D42")</f>
-        <v>12875</v>
+        <v>27418</v>
       </c>
       <c r="D9" s="1" cm="1">
         <f t="array" aca="1" ref="D9" ca="1">INDIRECT(B1&amp;"!G42")</f>
-        <v>12404</v>
+        <v>23625</v>
       </c>
       <c r="E9" s="1" cm="1">
         <f t="array" aca="1" ref="E9" ca="1">INDIRECT(B1&amp;"!D88")</f>
-        <v>13835</v>
+        <v>27981</v>
       </c>
       <c r="F9" s="1" cm="1">
         <f t="array" aca="1" ref="F9" ca="1">INDIRECT(B1&amp;"!G88")</f>
-        <v>11663</v>
+        <v>24069</v>
       </c>
       <c r="G9" s="1" cm="1">
         <f t="array" aca="1" ref="G9" ca="1">INDIRECT(B1&amp;"!D169")</f>
-        <v>13176</v>
+        <v>27615</v>
       </c>
       <c r="H9" s="1" cm="1">
         <f t="array" aca="1" ref="H9" ca="1">INDIRECT(B1&amp;"!G169")</f>
-        <v>12298</v>
+        <v>24213</v>
       </c>
       <c r="I9" s="1" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">INDIRECT(B1&amp;"!D210")</f>
-        <v>16012</v>
+        <v>33411</v>
       </c>
       <c r="J9" s="1" cm="1">
         <f t="array" aca="1" ref="J9" ca="1">INDIRECT(B1&amp;"!G210")</f>
-        <v>13091</v>
+        <v>25084</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="1"/>
@@ -27438,19 +27426,19 @@
       </c>
       <c r="M9" s="1">
         <f ca="1"/>
-        <v>12875</v>
+        <v>27418</v>
       </c>
       <c r="N9" s="1">
         <f ca="1"/>
-        <v>13835</v>
+        <v>27981</v>
       </c>
       <c r="O9" s="1">
         <f ca="1"/>
-        <v>13176</v>
+        <v>27615</v>
       </c>
       <c r="P9" s="1">
         <f ca="1"/>
-        <v>16012</v>
+        <v>33411</v>
       </c>
       <c r="R9" s="1">
         <f t="shared" si="2"/>
@@ -27458,19 +27446,19 @@
       </c>
       <c r="S9" s="1">
         <f ca="1"/>
-        <v>12404</v>
+        <v>23625</v>
       </c>
       <c r="T9" s="1">
         <f ca="1"/>
-        <v>11663</v>
+        <v>24069</v>
       </c>
       <c r="U9" s="1">
         <f ca="1"/>
-        <v>12298</v>
+        <v>24213</v>
       </c>
       <c r="V9" s="1">
         <f ca="1"/>
-        <v>13091</v>
+        <v>25084</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -27480,35 +27468,35 @@
       </c>
       <c r="C10" s="1" cm="1">
         <f t="array" aca="1" ref="C10" ca="1">INDIRECT(B1&amp;"!D43")</f>
-        <v>19400</v>
+        <v>39291</v>
       </c>
       <c r="D10" s="1" cm="1">
         <f t="array" aca="1" ref="D10" ca="1">INDIRECT(B1&amp;"!G43")</f>
-        <v>14614</v>
+        <v>29258</v>
       </c>
       <c r="E10" s="1" cm="1">
         <f t="array" aca="1" ref="E10" ca="1">INDIRECT(B1&amp;"!D89")</f>
-        <v>18945</v>
+        <v>40426</v>
       </c>
       <c r="F10" s="1" cm="1">
         <f t="array" aca="1" ref="F10" ca="1">INDIRECT(B1&amp;"!G89")</f>
-        <v>14158</v>
+        <v>27959</v>
       </c>
       <c r="G10" s="1" cm="1">
         <f t="array" aca="1" ref="G10" ca="1">INDIRECT(B1&amp;"!D171")</f>
-        <v>18825</v>
+        <v>40594</v>
       </c>
       <c r="H10" s="1" cm="1">
         <f t="array" aca="1" ref="H10" ca="1">INDIRECT(B1&amp;"!G171")</f>
-        <v>14661</v>
+        <v>28980</v>
       </c>
       <c r="I10" s="1" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">INDIRECT(B1&amp;"!D211")</f>
-        <v>21732</v>
+        <v>45841</v>
       </c>
       <c r="J10" s="1" cm="1">
         <f t="array" aca="1" ref="J10" ca="1">INDIRECT(B1&amp;"!G211")</f>
-        <v>15548</v>
+        <v>29629</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="1"/>
@@ -27516,19 +27504,19 @@
       </c>
       <c r="M10" s="1">
         <f ca="1"/>
-        <v>19400</v>
+        <v>39291</v>
       </c>
       <c r="N10" s="1">
         <f ca="1"/>
-        <v>18945</v>
+        <v>40426</v>
       </c>
       <c r="O10" s="1">
         <f ca="1"/>
-        <v>18825</v>
+        <v>40594</v>
       </c>
       <c r="P10" s="1">
         <f ca="1"/>
-        <v>21732</v>
+        <v>45841</v>
       </c>
       <c r="R10" s="1">
         <f t="shared" si="2"/>
@@ -27536,19 +27524,19 @@
       </c>
       <c r="S10" s="1">
         <f ca="1"/>
-        <v>14614</v>
+        <v>29258</v>
       </c>
       <c r="T10" s="1">
         <f ca="1"/>
-        <v>14158</v>
+        <v>27959</v>
       </c>
       <c r="U10" s="1">
         <f ca="1"/>
-        <v>14661</v>
+        <v>28980</v>
       </c>
       <c r="V10" s="1">
         <f ca="1"/>
-        <v>15548</v>
+        <v>29629</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -27558,35 +27546,35 @@
       </c>
       <c r="C11" s="1" cm="1">
         <f t="array" aca="1" ref="C11" ca="1">INDIRECT(B1&amp;"!D44")</f>
-        <v>24188</v>
+        <v>52039</v>
       </c>
       <c r="D11" s="1" cm="1">
         <f t="array" aca="1" ref="D11" ca="1">INDIRECT(B1&amp;"!G44")</f>
-        <v>17662</v>
+        <v>35314</v>
       </c>
       <c r="E11" s="1" cm="1">
         <f t="array" aca="1" ref="E11" ca="1">INDIRECT(B1&amp;"!D90")</f>
-        <v>23920</v>
+        <v>51825</v>
       </c>
       <c r="F11" s="1" cm="1">
         <f t="array" aca="1" ref="F11" ca="1">INDIRECT(B1&amp;"!G90")</f>
-        <v>16690</v>
+        <v>33992</v>
       </c>
       <c r="G11" s="1" cm="1">
         <f t="array" aca="1" ref="G11" ca="1">INDIRECT(B1&amp;"!D173")</f>
-        <v>23905</v>
+        <v>49939</v>
       </c>
       <c r="H11" s="1" cm="1">
         <f t="array" aca="1" ref="H11" ca="1">INDIRECT(B1&amp;"!G173")</f>
-        <v>17383</v>
+        <v>33915</v>
       </c>
       <c r="I11" s="1" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">INDIRECT(B1&amp;"!D212")</f>
-        <v>27103</v>
+        <v>56124</v>
       </c>
       <c r="J11" s="1" cm="1">
         <f t="array" aca="1" ref="J11" ca="1">INDIRECT(B1&amp;"!G212")</f>
-        <v>17736</v>
+        <v>33713</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" si="1"/>
@@ -27594,19 +27582,19 @@
       </c>
       <c r="M11" s="1">
         <f ca="1"/>
-        <v>24188</v>
+        <v>52039</v>
       </c>
       <c r="N11" s="1">
         <f ca="1"/>
-        <v>23920</v>
+        <v>51825</v>
       </c>
       <c r="O11" s="1">
         <f ca="1"/>
-        <v>23905</v>
+        <v>49939</v>
       </c>
       <c r="P11" s="1">
         <f ca="1"/>
-        <v>27103</v>
+        <v>56124</v>
       </c>
       <c r="R11" s="1">
         <f t="shared" si="2"/>
@@ -27614,19 +27602,19 @@
       </c>
       <c r="S11" s="1">
         <f ca="1"/>
-        <v>17662</v>
+        <v>35314</v>
       </c>
       <c r="T11" s="1">
         <f ca="1"/>
-        <v>16690</v>
+        <v>33992</v>
       </c>
       <c r="U11" s="1">
         <f ca="1"/>
-        <v>17383</v>
+        <v>33915</v>
       </c>
       <c r="V11" s="1">
         <f ca="1"/>
-        <v>17736</v>
+        <v>33713</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -27636,35 +27624,35 @@
       </c>
       <c r="C12" s="1" cm="1">
         <f t="array" aca="1" ref="C12" ca="1">INDIRECT(B1&amp;"!D45")</f>
-        <v>28344</v>
+        <v>60327</v>
       </c>
       <c r="D12" s="1" cm="1">
         <f t="array" aca="1" ref="D12" ca="1">INDIRECT(B1&amp;"!G45")</f>
-        <v>20410</v>
+        <v>40600</v>
       </c>
       <c r="E12" s="1" cm="1">
         <f t="array" aca="1" ref="E12" ca="1">INDIRECT(B1&amp;"!D91")</f>
-        <v>27520</v>
+        <v>61134</v>
       </c>
       <c r="F12" s="1" cm="1">
         <f t="array" aca="1" ref="F12" ca="1">INDIRECT(B1&amp;"!G91")</f>
-        <v>19008</v>
+        <v>39246</v>
       </c>
       <c r="G12" s="1" cm="1">
         <f t="array" aca="1" ref="G12" ca="1">INDIRECT(B1&amp;"!D175")</f>
-        <v>30373</v>
+        <v>65653</v>
       </c>
       <c r="H12" s="1" cm="1">
         <f t="array" aca="1" ref="H12" ca="1">INDIRECT(B1&amp;"!G175")</f>
-        <v>14769</v>
+        <v>39852</v>
       </c>
       <c r="I12" s="1" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">INDIRECT(B1&amp;"!D213")</f>
-        <v>33907</v>
+        <v>70674</v>
       </c>
       <c r="J12" s="1" cm="1">
         <f t="array" aca="1" ref="J12" ca="1">INDIRECT(B1&amp;"!G213")</f>
-        <v>20474</v>
+        <v>39174</v>
       </c>
       <c r="L12" s="1">
         <f t="shared" si="1"/>
@@ -27672,19 +27660,19 @@
       </c>
       <c r="M12" s="1">
         <f ca="1"/>
-        <v>28344</v>
+        <v>60327</v>
       </c>
       <c r="N12" s="1">
         <f ca="1"/>
-        <v>27520</v>
+        <v>61134</v>
       </c>
       <c r="O12" s="1">
         <f ca="1"/>
-        <v>30373</v>
+        <v>65653</v>
       </c>
       <c r="P12" s="1">
         <f ca="1"/>
-        <v>33907</v>
+        <v>70674</v>
       </c>
       <c r="R12" s="1">
         <f t="shared" si="2"/>
@@ -27692,19 +27680,19 @@
       </c>
       <c r="S12" s="1">
         <f ca="1"/>
-        <v>20410</v>
+        <v>40600</v>
       </c>
       <c r="T12" s="1">
         <f ca="1"/>
-        <v>19008</v>
+        <v>39246</v>
       </c>
       <c r="U12" s="1">
         <f ca="1"/>
-        <v>14769</v>
+        <v>39852</v>
       </c>
       <c r="V12" s="1">
         <f ca="1"/>
-        <v>20474</v>
+        <v>39174</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -27714,35 +27702,35 @@
       </c>
       <c r="C13" s="1" cm="1">
         <f t="array" aca="1" ref="C13" ca="1">INDIRECT(B1&amp;"!D46")</f>
-        <v>36510</v>
+        <v>78404</v>
       </c>
       <c r="D13" s="1" cm="1">
         <f t="array" aca="1" ref="D13" ca="1">INDIRECT(B1&amp;"!G46")</f>
-        <v>24803</v>
+        <v>49349</v>
       </c>
       <c r="E13" s="1" cm="1">
         <f t="array" aca="1" ref="E13" ca="1">INDIRECT(B1&amp;"!D92")</f>
-        <v>38057</v>
+        <v>81726</v>
       </c>
       <c r="F13" s="1" cm="1">
         <f t="array" aca="1" ref="F13" ca="1">INDIRECT(B1&amp;"!G92")</f>
-        <v>21444</v>
+        <v>45128</v>
       </c>
       <c r="G13" s="1" cm="1">
         <f t="array" aca="1" ref="G13" ca="1">INDIRECT(B1&amp;"!D176")</f>
-        <v>36939</v>
+        <v>79632</v>
       </c>
       <c r="H13" s="1" cm="1">
         <f t="array" aca="1" ref="H13" ca="1">INDIRECT(B1&amp;"!G176")</f>
-        <v>22707</v>
+        <v>44175</v>
       </c>
       <c r="I13" s="1" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">INDIRECT(B1&amp;"!D214")</f>
-        <v>47329</v>
+        <v>98879</v>
       </c>
       <c r="J13" s="1" cm="1">
         <f t="array" aca="1" ref="J13" ca="1">INDIRECT(B1&amp;"!G214")</f>
-        <v>22619</v>
+        <v>44859</v>
       </c>
       <c r="L13" s="1">
         <f t="shared" si="1"/>
@@ -27750,19 +27738,19 @@
       </c>
       <c r="M13" s="1">
         <f ca="1"/>
-        <v>36510</v>
+        <v>78404</v>
       </c>
       <c r="N13" s="1">
         <f ca="1"/>
-        <v>38057</v>
+        <v>81726</v>
       </c>
       <c r="O13" s="1">
         <f ca="1"/>
-        <v>36939</v>
+        <v>79632</v>
       </c>
       <c r="P13" s="1">
         <f ca="1"/>
-        <v>47329</v>
+        <v>98879</v>
       </c>
       <c r="R13" s="1">
         <f t="shared" si="2"/>
@@ -27770,19 +27758,19 @@
       </c>
       <c r="S13" s="1">
         <f ca="1"/>
-        <v>24803</v>
+        <v>49349</v>
       </c>
       <c r="T13" s="1">
         <f ca="1"/>
-        <v>21444</v>
+        <v>45128</v>
       </c>
       <c r="U13" s="1">
         <f ca="1"/>
-        <v>22707</v>
+        <v>44175</v>
       </c>
       <c r="V13" s="1">
         <f ca="1"/>
-        <v>22619</v>
+        <v>44859</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -27792,35 +27780,35 @@
       </c>
       <c r="C14" s="1" cm="1">
         <f t="array" aca="1" ref="C14" ca="1">INDIRECT(B1&amp;"!D47")</f>
-        <v>50887</v>
+        <v>112258</v>
       </c>
       <c r="D14" s="1" cm="1">
         <f t="array" aca="1" ref="D14" ca="1">INDIRECT(B1&amp;"!G47")</f>
-        <v>29327</v>
+        <v>56502</v>
       </c>
       <c r="E14" s="1" cm="1">
         <f t="array" aca="1" ref="E14" ca="1">INDIRECT(B1&amp;"!D93")</f>
-        <v>51263</v>
+        <v>119800</v>
       </c>
       <c r="F14" s="1" cm="1">
         <f t="array" aca="1" ref="F14" ca="1">INDIRECT(B1&amp;"!G93")</f>
-        <v>23923</v>
+        <v>48906</v>
       </c>
       <c r="G14" s="1" cm="1">
         <f t="array" aca="1" ref="G14" ca="1">INDIRECT(B1&amp;"!D177")</f>
-        <v>52918</v>
+        <v>112751</v>
       </c>
       <c r="H14" s="1" cm="1">
         <f t="array" aca="1" ref="H14" ca="1">INDIRECT(B1&amp;"!G177")</f>
-        <v>24623</v>
+        <v>49696</v>
       </c>
       <c r="I14" s="1" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">INDIRECT(B1&amp;"!D215")</f>
-        <v>78160</v>
+        <v>160899</v>
       </c>
       <c r="J14" s="1" cm="1">
         <f t="array" aca="1" ref="J14" ca="1">INDIRECT(B1&amp;"!G215")</f>
-        <v>26300</v>
+        <v>51248</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="1">
@@ -27829,19 +27817,19 @@
       </c>
       <c r="M14" s="1">
         <f ca="1"/>
-        <v>50887</v>
+        <v>112258</v>
       </c>
       <c r="N14" s="1">
         <f ca="1"/>
-        <v>51263</v>
+        <v>119800</v>
       </c>
       <c r="O14" s="1">
         <f ca="1"/>
-        <v>52918</v>
+        <v>112751</v>
       </c>
       <c r="P14" s="1">
         <f ca="1"/>
-        <v>78160</v>
+        <v>160899</v>
       </c>
       <c r="R14" s="1">
         <f t="shared" si="2"/>
@@ -27849,19 +27837,19 @@
       </c>
       <c r="S14" s="1">
         <f ca="1"/>
-        <v>29327</v>
+        <v>56502</v>
       </c>
       <c r="T14" s="1">
         <f ca="1"/>
-        <v>23923</v>
+        <v>48906</v>
       </c>
       <c r="U14" s="1">
         <f ca="1"/>
-        <v>24623</v>
+        <v>49696</v>
       </c>
       <c r="V14" s="1">
         <f ca="1"/>
-        <v>26300</v>
+        <v>51248</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -27937,73 +27925,73 @@
       </c>
       <c r="C18" s="3" cm="1">
         <f t="array" aca="1" ref="C18" ca="1">INDIRECT(B1&amp;"!C34")</f>
-        <v>63</v>
+        <v>126</v>
       </c>
       <c r="D18" s="3" cm="1">
         <f t="array" aca="1" ref="D18" ca="1">INDIRECT(B1&amp;"!F34")</f>
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="E18" s="1" cm="1">
         <f t="array" aca="1" ref="E18" ca="1">INDIRECT(B1&amp;"!C78")</f>
-        <v>58</v>
+        <v>124</v>
       </c>
       <c r="F18" s="1" cm="1">
         <f t="array" aca="1" ref="F18" ca="1">INDIRECT(B1&amp;"!F78")</f>
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="G18" s="1" cm="1">
         <f t="array" aca="1" ref="G18" ca="1">INDIRECT(B1&amp;"!C161")</f>
-        <v>61</v>
+        <v>127</v>
       </c>
       <c r="H18" s="1" cm="1">
         <f t="array" aca="1" ref="H18" ca="1">INDIRECT(B1&amp;"!F161")</f>
-        <v>61</v>
+        <v>125</v>
       </c>
       <c r="I18" s="1" cm="1">
         <f t="array" aca="1" ref="I18" ca="1">INDIRECT(B1&amp;"!C206")</f>
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="J18" s="1" cm="1">
         <f t="array" aca="1" ref="J18" ca="1">INDIRECT(B1&amp;"!F206")</f>
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="L18" s="1">
         <v>100000</v>
       </c>
       <c r="M18" s="1" cm="1">
         <f t="array" aca="1" ref="M18:M27" ca="1">C18:C27</f>
-        <v>63</v>
+        <v>126</v>
       </c>
       <c r="N18" s="1" cm="1">
         <f t="array" aca="1" ref="N18:N27" ca="1">E18:E27</f>
-        <v>58</v>
+        <v>124</v>
       </c>
       <c r="O18" s="1" cm="1">
         <f t="array" aca="1" ref="O18:O27" ca="1">G18:G27</f>
-        <v>61</v>
+        <v>127</v>
       </c>
       <c r="P18" s="1" cm="1">
         <f t="array" aca="1" ref="P18:P27" ca="1">I18:I27</f>
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="R18" s="1">
         <v>100000</v>
       </c>
       <c r="S18" s="1" cm="1">
         <f t="array" aca="1" ref="S18:S27" ca="1">D18:D27</f>
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="T18" s="1" cm="1">
         <f t="array" aca="1" ref="T18:T27" ca="1">F18:F27</f>
-        <v>59</v>
+        <v>123</v>
       </c>
       <c r="U18" s="1" cm="1">
         <f t="array" aca="1" ref="U18:U27" ca="1">H18:H27</f>
-        <v>61</v>
+        <v>125</v>
       </c>
       <c r="V18" s="1" cm="1">
         <f t="array" aca="1" ref="V18:V27" ca="1">J18:J27</f>
-        <v>55</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.25">
@@ -28013,35 +28001,35 @@
       </c>
       <c r="C19" s="1" cm="1">
         <f t="array" aca="1" ref="C19" ca="1">INDIRECT(B1&amp;"!C39")</f>
-        <v>57</v>
+        <v>123</v>
       </c>
       <c r="D19" s="1" cm="1">
         <f t="array" aca="1" ref="D19" ca="1">INDIRECT(B1&amp;"!F39")</f>
-        <v>55</v>
+        <v>118</v>
       </c>
       <c r="E19" s="1" cm="1">
         <f t="array" aca="1" ref="E19" ca="1">INDIRECT(B1&amp;"!C81")</f>
-        <v>58</v>
+        <v>121</v>
       </c>
       <c r="F19" s="1" cm="1">
         <f t="array" aca="1" ref="F19" ca="1">INDIRECT(B1&amp;"!F81")</f>
-        <v>49</v>
+        <v>124</v>
       </c>
       <c r="G19" s="1" cm="1">
         <f t="array" aca="1" ref="G19" ca="1">INDIRECT(B1&amp;"!C163")</f>
-        <v>58</v>
+        <v>124</v>
       </c>
       <c r="H19" s="1" cm="1">
         <f t="array" aca="1" ref="H19" ca="1">INDIRECT(B1&amp;"!F163")</f>
-        <v>61</v>
+        <v>123</v>
       </c>
       <c r="I19" s="1" cm="1">
         <f t="array" aca="1" ref="I19" ca="1">INDIRECT(B1&amp;"!C207")</f>
-        <v>59</v>
+        <v>124</v>
       </c>
       <c r="J19" s="1" cm="1">
         <f t="array" aca="1" ref="J19" ca="1">INDIRECT(B1&amp;"!F207")</f>
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="L19" s="1">
         <f>L18 + 100000</f>
@@ -28049,19 +28037,19 @@
       </c>
       <c r="M19" s="1">
         <f ca="1"/>
-        <v>57</v>
+        <v>123</v>
       </c>
       <c r="N19" s="1">
         <f ca="1"/>
-        <v>58</v>
+        <v>121</v>
       </c>
       <c r="O19" s="1">
         <f ca="1"/>
-        <v>58</v>
+        <v>124</v>
       </c>
       <c r="P19" s="1">
         <f ca="1"/>
-        <v>59</v>
+        <v>124</v>
       </c>
       <c r="R19" s="1">
         <f>R18 + 100000</f>
@@ -28069,19 +28057,19 @@
       </c>
       <c r="S19" s="1">
         <f ca="1"/>
-        <v>55</v>
+        <v>118</v>
       </c>
       <c r="T19" s="1">
         <f ca="1"/>
-        <v>49</v>
+        <v>124</v>
       </c>
       <c r="U19" s="1">
         <f ca="1"/>
-        <v>61</v>
+        <v>123</v>
       </c>
       <c r="V19" s="1">
         <f ca="1"/>
-        <v>48</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.25">
@@ -28091,35 +28079,35 @@
       </c>
       <c r="C20" s="1" cm="1">
         <f t="array" aca="1" ref="C20" ca="1">INDIRECT(B1&amp;"!C40")</f>
-        <v>54</v>
+        <v>122</v>
       </c>
       <c r="D20" s="1" cm="1">
         <f t="array" aca="1" ref="D20" ca="1">INDIRECT(B1&amp;"!F40")</f>
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="E20" s="1" cm="1">
         <f t="array" aca="1" ref="E20" ca="1">INDIRECT(B1&amp;"!C84")</f>
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="F20" s="1" cm="1">
         <f t="array" aca="1" ref="F20" ca="1">INDIRECT(B1&amp;"!F84")</f>
-        <v>55</v>
+        <v>119</v>
       </c>
       <c r="G20" s="1" cm="1">
         <f t="array" aca="1" ref="G20" ca="1">INDIRECT(B1&amp;"!C165")</f>
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="H20" s="1" cm="1">
         <f t="array" aca="1" ref="H20" ca="1">INDIRECT(B1&amp;"!F165")</f>
-        <v>57</v>
+        <v>120</v>
       </c>
       <c r="I20" s="1" cm="1">
         <f t="array" aca="1" ref="I20" ca="1">INDIRECT(B1&amp;"!C208")</f>
-        <v>57</v>
+        <v>121</v>
       </c>
       <c r="J20" s="1" cm="1">
         <f t="array" aca="1" ref="J20" ca="1">INDIRECT(B1&amp;"!F208")</f>
-        <v>57</v>
+        <v>123</v>
       </c>
       <c r="L20" s="1">
         <f t="shared" ref="L20:L27" si="4">L19 + 100000</f>
@@ -28127,19 +28115,19 @@
       </c>
       <c r="M20" s="1">
         <f ca="1"/>
-        <v>54</v>
+        <v>122</v>
       </c>
       <c r="N20" s="1">
         <f ca="1"/>
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="O20" s="1">
         <f ca="1"/>
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="P20" s="1">
         <f ca="1"/>
-        <v>57</v>
+        <v>121</v>
       </c>
       <c r="R20" s="1">
         <f t="shared" ref="R20:R27" si="5">R19 + 100000</f>
@@ -28147,19 +28135,19 @@
       </c>
       <c r="S20" s="1">
         <f ca="1"/>
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="T20" s="1">
         <f ca="1"/>
-        <v>55</v>
+        <v>119</v>
       </c>
       <c r="U20" s="1">
         <f ca="1"/>
-        <v>57</v>
+        <v>120</v>
       </c>
       <c r="V20" s="1">
         <f ca="1"/>
-        <v>57</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.25">
@@ -28169,35 +28157,35 @@
       </c>
       <c r="C21" s="1" cm="1">
         <f t="array" aca="1" ref="C21" ca="1">INDIRECT(B1&amp;"!C41")</f>
-        <v>55</v>
+        <v>119</v>
       </c>
       <c r="D21" s="1" cm="1">
         <f t="array" aca="1" ref="D21" ca="1">INDIRECT(B1&amp;"!F41")</f>
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="E21" s="1" cm="1">
         <f t="array" aca="1" ref="E21" ca="1">INDIRECT(B1&amp;"!C87")</f>
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="F21" s="1" cm="1">
         <f t="array" aca="1" ref="F21" ca="1">INDIRECT(B1&amp;"!F87")</f>
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="G21" s="1" cm="1">
         <f t="array" aca="1" ref="G21" ca="1">INDIRECT(B1&amp;"!C167")</f>
-        <v>54</v>
+        <v>120</v>
       </c>
       <c r="H21" s="1" cm="1">
         <f t="array" aca="1" ref="H21" ca="1">INDIRECT(B1&amp;"!F167")</f>
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="I21" s="1" cm="1">
         <f t="array" aca="1" ref="I21" ca="1">INDIRECT(B1&amp;"!C209")</f>
-        <v>57</v>
+        <v>120</v>
       </c>
       <c r="J21" s="1" cm="1">
         <f t="array" aca="1" ref="J21" ca="1">INDIRECT(B1&amp;"!F209")</f>
-        <v>56</v>
+        <v>120</v>
       </c>
       <c r="L21" s="1">
         <f t="shared" si="4"/>
@@ -28205,19 +28193,19 @@
       </c>
       <c r="M21" s="1">
         <f ca="1"/>
-        <v>55</v>
+        <v>119</v>
       </c>
       <c r="N21" s="1">
         <f ca="1"/>
-        <v>54</v>
+        <v>116</v>
       </c>
       <c r="O21" s="1">
         <f ca="1"/>
-        <v>54</v>
+        <v>120</v>
       </c>
       <c r="P21" s="1">
         <f ca="1"/>
-        <v>57</v>
+        <v>120</v>
       </c>
       <c r="R21" s="1">
         <f t="shared" si="5"/>
@@ -28225,19 +28213,19 @@
       </c>
       <c r="S21" s="1">
         <f ca="1"/>
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="T21" s="1">
         <f ca="1"/>
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="U21" s="1">
         <f ca="1"/>
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="V21" s="1">
         <f ca="1"/>
-        <v>56</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.25">
@@ -28247,35 +28235,35 @@
       </c>
       <c r="C22" s="1" cm="1">
         <f t="array" aca="1" ref="C22" ca="1">INDIRECT(B1&amp;"!C42")</f>
-        <v>52</v>
+        <v>119</v>
       </c>
       <c r="D22" s="1" cm="1">
         <f t="array" aca="1" ref="D22" ca="1">INDIRECT(B1&amp;"!F42")</f>
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="E22" s="1" cm="1">
         <f t="array" aca="1" ref="E22" ca="1">INDIRECT(B1&amp;"!C88")</f>
-        <v>55</v>
+        <v>117</v>
       </c>
       <c r="F22" s="1" cm="1">
         <f t="array" aca="1" ref="F22" ca="1">INDIRECT(B1&amp;"!F88")</f>
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="G22" s="1" cm="1">
         <f t="array" aca="1" ref="G22" ca="1">INDIRECT(B1&amp;"!C169")</f>
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="H22" s="1" cm="1">
         <f t="array" aca="1" ref="H22" ca="1">INDIRECT(B1&amp;"!F169")</f>
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="I22" s="1" cm="1">
         <f t="array" aca="1" ref="I22" ca="1">INDIRECT(B1&amp;"!C210")</f>
-        <v>57</v>
+        <v>120</v>
       </c>
       <c r="J22" s="1" cm="1">
         <f t="array" aca="1" ref="J22" ca="1">INDIRECT(B1&amp;"!F210")</f>
-        <v>56</v>
+        <v>119</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" si="4"/>
@@ -28283,19 +28271,19 @@
       </c>
       <c r="M22" s="1">
         <f ca="1"/>
-        <v>52</v>
+        <v>119</v>
       </c>
       <c r="N22" s="1">
         <f ca="1"/>
-        <v>55</v>
+        <v>117</v>
       </c>
       <c r="O22" s="1">
         <f ca="1"/>
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="P22" s="1">
         <f ca="1"/>
-        <v>57</v>
+        <v>120</v>
       </c>
       <c r="R22" s="1">
         <f t="shared" si="5"/>
@@ -28303,19 +28291,19 @@
       </c>
       <c r="S22" s="1">
         <f ca="1"/>
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="T22" s="1">
         <f ca="1"/>
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="U22" s="1">
         <f ca="1"/>
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="V22" s="1">
         <f ca="1"/>
-        <v>56</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
@@ -28325,35 +28313,35 @@
       </c>
       <c r="C23" s="1" cm="1">
         <f t="array" aca="1" ref="C23" ca="1">INDIRECT(B1&amp;"!C43")</f>
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="D23" s="1" cm="1">
         <f t="array" aca="1" ref="D23" ca="1">INDIRECT(B1&amp;"!F43")</f>
-        <v>55</v>
+        <v>115</v>
       </c>
       <c r="E23" s="1" cm="1">
         <f t="array" aca="1" ref="E23" ca="1">INDIRECT(B1&amp;"!C89")</f>
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="F23" s="1" cm="1">
         <f t="array" aca="1" ref="F23" ca="1">INDIRECT(B1&amp;"!F89")</f>
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="G23" s="1" cm="1">
         <f t="array" aca="1" ref="G23" ca="1">INDIRECT(B1&amp;"!C171")</f>
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="H23" s="1" cm="1">
         <f t="array" aca="1" ref="H23" ca="1">INDIRECT(B1&amp;"!F171")</f>
-        <v>52</v>
+        <v>117</v>
       </c>
       <c r="I23" s="1" cm="1">
         <f t="array" aca="1" ref="I23" ca="1">INDIRECT(B1&amp;"!C211")</f>
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="J23" s="1" cm="1">
         <f t="array" aca="1" ref="J23" ca="1">INDIRECT(B1&amp;"!F211")</f>
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="L23" s="1">
         <f t="shared" si="4"/>
@@ -28361,19 +28349,19 @@
       </c>
       <c r="M23" s="1">
         <f ca="1"/>
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="N23" s="1">
         <f ca="1"/>
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="O23" s="1">
         <f ca="1"/>
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="P23" s="1">
         <f ca="1"/>
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="R23" s="1">
         <f t="shared" si="5"/>
@@ -28381,19 +28369,19 @@
       </c>
       <c r="S23" s="1">
         <f ca="1"/>
-        <v>55</v>
+        <v>115</v>
       </c>
       <c r="T23" s="1">
         <f ca="1"/>
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="U23" s="1">
         <f ca="1"/>
-        <v>52</v>
+        <v>117</v>
       </c>
       <c r="V23" s="1">
         <f ca="1"/>
-        <v>55</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="2:22" x14ac:dyDescent="0.25">
@@ -28403,35 +28391,35 @@
       </c>
       <c r="C24" s="1" cm="1">
         <f t="array" aca="1" ref="C24" ca="1">INDIRECT(B1&amp;"!C44")</f>
-        <v>54</v>
+        <v>120</v>
       </c>
       <c r="D24" s="1" cm="1">
         <f t="array" aca="1" ref="D24" ca="1">INDIRECT(B1&amp;"!F44")</f>
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="E24" s="1" cm="1">
         <f t="array" aca="1" ref="E24" ca="1">INDIRECT(B1&amp;"!C90")</f>
-        <v>52</v>
+        <v>115</v>
       </c>
       <c r="F24" s="1" cm="1">
         <f t="array" aca="1" ref="F24" ca="1">INDIRECT(B1&amp;"!F90")</f>
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="G24" s="1" cm="1">
         <f t="array" aca="1" ref="G24" ca="1">INDIRECT(B1&amp;"!C173")</f>
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="H24" s="1" cm="1">
         <f t="array" aca="1" ref="H24" ca="1">INDIRECT(B1&amp;"!F173")</f>
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="I24" s="1" cm="1">
         <f t="array" aca="1" ref="I24" ca="1">INDIRECT(B1&amp;"!C212")</f>
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="J24" s="1" cm="1">
         <f t="array" aca="1" ref="J24" ca="1">INDIRECT(B1&amp;"!F212")</f>
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="L24" s="1">
         <f t="shared" si="4"/>
@@ -28439,19 +28427,19 @@
       </c>
       <c r="M24" s="1">
         <f ca="1"/>
-        <v>54</v>
+        <v>120</v>
       </c>
       <c r="N24" s="1">
         <f ca="1"/>
-        <v>52</v>
+        <v>115</v>
       </c>
       <c r="O24" s="1">
         <f ca="1"/>
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="P24" s="1">
         <f ca="1"/>
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="R24" s="1">
         <f t="shared" si="5"/>
@@ -28459,19 +28447,19 @@
       </c>
       <c r="S24" s="1">
         <f ca="1"/>
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="T24" s="1">
         <f ca="1"/>
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="U24" s="1">
         <f ca="1"/>
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="V24" s="1">
         <f ca="1"/>
-        <v>53</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.25">
@@ -28481,35 +28469,35 @@
       </c>
       <c r="C25" s="1" cm="1">
         <f t="array" aca="1" ref="C25" ca="1">INDIRECT(B1&amp;"!C45")</f>
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="D25" s="1" cm="1">
         <f t="array" aca="1" ref="D25" ca="1">INDIRECT(B1&amp;"!F45")</f>
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="E25" s="1" cm="1">
         <f t="array" aca="1" ref="E25" ca="1">INDIRECT(B1&amp;"!C91")</f>
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="F25" s="1" cm="1">
         <f t="array" aca="1" ref="F25" ca="1">INDIRECT(B1&amp;"!F91")</f>
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="G25" s="1" cm="1">
         <f t="array" aca="1" ref="G25" ca="1">INDIRECT(B1&amp;"!C175")</f>
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="H25" s="1" cm="1">
         <f t="array" aca="1" ref="H25" ca="1">INDIRECT(B1&amp;"!F175")</f>
-        <v>49</v>
+        <v>117</v>
       </c>
       <c r="I25" s="1" cm="1">
         <f t="array" aca="1" ref="I25" ca="1">INDIRECT(B1&amp;"!C213")</f>
-        <v>52</v>
+        <v>118</v>
       </c>
       <c r="J25" s="1" cm="1">
         <f t="array" aca="1" ref="J25" ca="1">INDIRECT(B1&amp;"!F213")</f>
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="L25" s="1">
         <f t="shared" si="4"/>
@@ -28517,19 +28505,19 @@
       </c>
       <c r="M25" s="1">
         <f ca="1"/>
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="N25" s="1">
         <f ca="1"/>
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="O25" s="1">
         <f ca="1"/>
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="P25" s="1">
         <f ca="1"/>
-        <v>52</v>
+        <v>118</v>
       </c>
       <c r="R25" s="1">
         <f t="shared" si="5"/>
@@ -28537,19 +28525,19 @@
       </c>
       <c r="S25" s="1">
         <f ca="1"/>
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="T25" s="1">
         <f ca="1"/>
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="U25" s="1">
         <f ca="1"/>
-        <v>49</v>
+        <v>117</v>
       </c>
       <c r="V25" s="1">
         <f ca="1"/>
-        <v>53</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.25">
@@ -28559,35 +28547,35 @@
       </c>
       <c r="C26" s="1" cm="1">
         <f t="array" aca="1" ref="C26" ca="1">INDIRECT(B1&amp;"!C46")</f>
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="D26" s="1" cm="1">
         <f t="array" aca="1" ref="D26" ca="1">INDIRECT(B1&amp;"!F46")</f>
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="E26" s="1" cm="1">
         <f t="array" aca="1" ref="E26" ca="1">INDIRECT(B1&amp;"!C92")</f>
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="F26" s="1" cm="1">
         <f t="array" aca="1" ref="F26" ca="1">INDIRECT(B1&amp;"!F92")</f>
-        <v>51</v>
+        <v>115</v>
       </c>
       <c r="G26" s="1" cm="1">
         <f t="array" aca="1" ref="G26" ca="1">INDIRECT(B1&amp;"!C176")</f>
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="H26" s="1" cm="1">
         <f t="array" aca="1" ref="H26" ca="1">INDIRECT(B1&amp;"!F176")</f>
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="I26" s="1" cm="1">
         <f t="array" aca="1" ref="I26" ca="1">INDIRECT(B1&amp;"!C214")</f>
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="J26" s="1" cm="1">
         <f t="array" aca="1" ref="J26" ca="1">INDIRECT(B1&amp;"!F214")</f>
-        <v>52</v>
+        <v>118</v>
       </c>
       <c r="L26" s="1">
         <f t="shared" si="4"/>
@@ -28595,19 +28583,19 @@
       </c>
       <c r="M26" s="1">
         <f ca="1"/>
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="N26" s="1">
         <f ca="1"/>
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="O26" s="1">
         <f ca="1"/>
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="P26" s="1">
         <f ca="1"/>
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="R26" s="1">
         <f t="shared" si="5"/>
@@ -28615,19 +28603,19 @@
       </c>
       <c r="S26" s="1">
         <f ca="1"/>
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="T26" s="1">
         <f ca="1"/>
-        <v>51</v>
+        <v>115</v>
       </c>
       <c r="U26" s="1">
         <f ca="1"/>
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="V26" s="1">
         <f ca="1"/>
-        <v>52</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.25">
@@ -28637,35 +28625,35 @@
       </c>
       <c r="C27" s="1" cm="1">
         <f t="array" aca="1" ref="C27" ca="1">INDIRECT(B1&amp;"!C47")</f>
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="D27" s="1" cm="1">
         <f t="array" aca="1" ref="D27" ca="1">INDIRECT(B1&amp;"!F47")</f>
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="E27" s="1" cm="1">
         <f t="array" aca="1" ref="E27" ca="1">INDIRECT(B1&amp;"!C93")</f>
-        <v>51</v>
+        <v>115</v>
       </c>
       <c r="F27" s="1" cm="1">
         <f t="array" aca="1" ref="F27" ca="1">INDIRECT(B1&amp;"!F93")</f>
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="G27" s="1" cm="1">
         <f t="array" aca="1" ref="G27" ca="1">INDIRECT(B1&amp;"!C177")</f>
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="H27" s="1" cm="1">
         <f t="array" aca="1" ref="H27" ca="1">INDIRECT(B1&amp;"!F177")</f>
-        <v>52</v>
+        <v>117</v>
       </c>
       <c r="I27" s="1" cm="1">
         <f t="array" aca="1" ref="I27" ca="1">INDIRECT(B1&amp;"!C215")</f>
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="J27" s="1" cm="1">
         <f t="array" aca="1" ref="J27" ca="1">INDIRECT(B1&amp;"!F215")</f>
-        <v>52</v>
+        <v>117</v>
       </c>
       <c r="L27" s="1">
         <f t="shared" si="4"/>
@@ -28673,19 +28661,19 @@
       </c>
       <c r="M27" s="1">
         <f ca="1"/>
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="N27" s="1">
         <f ca="1"/>
-        <v>51</v>
+        <v>115</v>
       </c>
       <c r="O27" s="1">
         <f ca="1"/>
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="P27" s="1">
         <f ca="1"/>
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="R27" s="1">
         <f t="shared" si="5"/>
@@ -28693,80 +28681,55 @@
       </c>
       <c r="S27" s="1">
         <f ca="1"/>
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="T27" s="1">
         <f ca="1"/>
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="U27" s="1">
         <f ca="1"/>
-        <v>52</v>
+        <v>117</v>
       </c>
       <c r="V27" s="1">
         <f ca="1"/>
-        <v>52</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="N31" s="1"/>
-      <c r="O31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="L32" t="s">
-        <v>40</v>
-      </c>
-      <c r="M32" s="6">
-        <f ca="1">AVERAGE(C5,E5,G5,I5)</f>
-        <v>2340.5</v>
-      </c>
-      <c r="N32" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O32" s="1">
-        <f>(126)</f>
-        <v>126</v>
-      </c>
-      <c r="P32" s="1"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
     </row>
     <row r="33" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L33" t="s">
-        <v>41</v>
-      </c>
-      <c r="M33" s="6">
-        <f ca="1">AVERAGE(D5,F5,H5,J5)</f>
-        <v>3787</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
     </row>
     <row r="34" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M34">
-        <v>0.66</v>
-      </c>
-      <c r="N34" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
     </row>
     <row r="35" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="M35">
-        <v>2844.6</v>
-      </c>
-      <c r="N35" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28808,7 +28771,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -28886,7 +28849,7 @@
         <v>39</v>
       </c>
       <c r="O4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -28964,7 +28927,7 @@
         <f>AVERAGE(I4:L4)</f>
         <v>6483.5</v>
       </c>
-      <c r="O6" s="16"/>
+      <c r="O6" s="15"/>
     </row>
     <row r="7" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -29073,7 +29036,7 @@
         <f>AVERAGE(I13:L13)</f>
         <v>51588</v>
       </c>
-      <c r="O9" s="16"/>
+      <c r="O9" s="15"/>
     </row>
     <row r="10" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
@@ -29205,7 +29168,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -29283,7 +29246,7 @@
         <v>39</v>
       </c>
       <c r="O18" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29361,7 +29324,7 @@
         <f>AVERAGE(I18:L18)</f>
         <v>5728.75</v>
       </c>
-      <c r="O20" s="16"/>
+      <c r="O20" s="15"/>
     </row>
     <row r="21" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
@@ -29470,7 +29433,7 @@
         <f>AVERAGE(I27:L27)</f>
         <v>43597.75</v>
       </c>
-      <c r="O23" s="16"/>
+      <c r="O23" s="15"/>
     </row>
     <row r="24" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
@@ -29602,7 +29565,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -29680,7 +29643,7 @@
         <v>39</v>
       </c>
       <c r="O32" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -29758,7 +29721,7 @@
         <f>AVERAGE(I32:L32)</f>
         <v>3787</v>
       </c>
-      <c r="O34" s="16"/>
+      <c r="O34" s="15"/>
     </row>
     <row r="35" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
@@ -29867,7 +29830,7 @@
         <f>AVERAGE(I41:L41)</f>
         <v>26043.25</v>
       </c>
-      <c r="O37" s="16"/>
+      <c r="O37" s="15"/>
     </row>
     <row r="38" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
@@ -29999,252 +29962,252 @@
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E45" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F45" s="8" t="s">
+      <c r="F45" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" s="9">
+        <v>4205</v>
+      </c>
+      <c r="D46" s="9">
+        <v>3842</v>
+      </c>
+      <c r="E46" s="9">
+        <v>4775</v>
+      </c>
+      <c r="F46" s="9">
+        <v>4417</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B47" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="9">
+        <v>5291</v>
+      </c>
+      <c r="D47" s="9">
+        <v>5630</v>
+      </c>
+      <c r="E47" s="9">
+        <v>7153</v>
+      </c>
+      <c r="F47" s="9">
+        <v>7860</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B48" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" s="12">
+        <v>2910</v>
+      </c>
+      <c r="D48" s="12">
+        <v>3243</v>
+      </c>
+      <c r="E48" s="12">
+        <v>3634</v>
+      </c>
+      <c r="F48" s="12">
+        <v>2805</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="12">
+        <v>4331</v>
+      </c>
+      <c r="D49" s="12">
+        <v>4846</v>
+      </c>
+      <c r="E49" s="12">
+        <v>6197</v>
+      </c>
+      <c r="F49" s="12">
+        <v>7541</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C46" s="10">
-        <v>4205</v>
-      </c>
-      <c r="D46" s="10">
-        <v>3842</v>
-      </c>
-      <c r="E46" s="10">
-        <v>4775</v>
-      </c>
-      <c r="F46" s="10">
-        <v>4417</v>
-      </c>
-    </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="11" t="s">
+      <c r="C50" s="14">
+        <v>2364</v>
+      </c>
+      <c r="D50" s="14">
+        <v>2297</v>
+      </c>
+      <c r="E50" s="14">
+        <v>2313</v>
+      </c>
+      <c r="F50" s="14">
+        <v>2388</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C47" s="10">
-        <v>5291</v>
-      </c>
-      <c r="D47" s="10">
-        <v>5630</v>
-      </c>
-      <c r="E47" s="10">
-        <v>7153</v>
-      </c>
-      <c r="F47" s="10">
-        <v>7860</v>
-      </c>
-    </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C48" s="13">
-        <v>2910</v>
-      </c>
-      <c r="D48" s="13">
-        <v>3243</v>
-      </c>
-      <c r="E48" s="13">
-        <v>3634</v>
-      </c>
-      <c r="F48" s="13">
-        <v>2805</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="12" t="s">
+      <c r="C51" s="14">
+        <v>3551</v>
+      </c>
+      <c r="D51" s="14">
+        <v>3287</v>
+      </c>
+      <c r="E51" s="14">
+        <v>3925</v>
+      </c>
+      <c r="F51" s="14">
+        <v>4385</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="16"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="16" t="s">
         <v>51</v>
-      </c>
-      <c r="C49" s="13">
-        <v>4331</v>
-      </c>
-      <c r="D49" s="13">
-        <v>4846</v>
-      </c>
-      <c r="E49" s="13">
-        <v>6197</v>
-      </c>
-      <c r="F49" s="13">
-        <v>7541</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C50" s="15">
-        <v>2364</v>
-      </c>
-      <c r="D50" s="15">
-        <v>2297</v>
-      </c>
-      <c r="E50" s="15">
-        <v>2313</v>
-      </c>
-      <c r="F50" s="15">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C51" s="15">
-        <v>3551</v>
-      </c>
-      <c r="D51" s="15">
-        <v>3287</v>
-      </c>
-      <c r="E51" s="15">
-        <v>3925</v>
-      </c>
-      <c r="F51" s="15">
-        <v>4385</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="17"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="17" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
-      <c r="C54" s="7" t="s">
+      <c r="C54" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="D54" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="E54" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F54" s="8" t="s">
+      <c r="F54" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B55" s="11" t="s">
+      <c r="B55" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C55" s="9">
+        <v>112258</v>
+      </c>
+      <c r="D55" s="9">
+        <v>119800</v>
+      </c>
+      <c r="E55" s="9">
+        <v>112751</v>
+      </c>
+      <c r="F55" s="9">
+        <v>160899</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" s="9">
+        <v>56502</v>
+      </c>
+      <c r="D56" s="9">
+        <v>48906</v>
+      </c>
+      <c r="E56" s="9">
+        <v>49696</v>
+      </c>
+      <c r="F56" s="9">
+        <v>51248</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C57" s="12">
+        <v>102709</v>
+      </c>
+      <c r="D57" s="12">
+        <v>103364</v>
+      </c>
+      <c r="E57" s="12">
+        <v>102856</v>
+      </c>
+      <c r="F57" s="12">
+        <v>131270</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C58" s="12">
+        <v>48322</v>
+      </c>
+      <c r="D58" s="12">
+        <v>39878</v>
+      </c>
+      <c r="E58" s="12">
+        <v>36861</v>
+      </c>
+      <c r="F58" s="12">
+        <v>49330</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C55" s="10">
-        <v>112258</v>
-      </c>
-      <c r="D55" s="10">
-        <v>119800</v>
-      </c>
-      <c r="E55" s="10">
-        <v>112751</v>
-      </c>
-      <c r="F55" s="10">
-        <v>160899</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B56" s="11" t="s">
+      <c r="C59" s="14">
+        <v>50887</v>
+      </c>
+      <c r="D59" s="14">
+        <v>51263</v>
+      </c>
+      <c r="E59" s="14">
+        <v>52918</v>
+      </c>
+      <c r="F59" s="14">
+        <v>78160</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C56" s="10">
-        <v>56502</v>
-      </c>
-      <c r="D56" s="10">
-        <v>48906</v>
-      </c>
-      <c r="E56" s="10">
-        <v>49696</v>
-      </c>
-      <c r="F56" s="10">
-        <v>51248</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C57" s="13">
-        <v>102709</v>
-      </c>
-      <c r="D57" s="13">
-        <v>103364</v>
-      </c>
-      <c r="E57" s="13">
-        <v>102856</v>
-      </c>
-      <c r="F57" s="13">
-        <v>131270</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C58" s="13">
-        <v>48322</v>
-      </c>
-      <c r="D58" s="13">
-        <v>39878</v>
-      </c>
-      <c r="E58" s="13">
-        <v>36861</v>
-      </c>
-      <c r="F58" s="13">
-        <v>49330</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B59" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C59" s="15">
-        <v>50887</v>
-      </c>
-      <c r="D59" s="15">
-        <v>51263</v>
-      </c>
-      <c r="E59" s="15">
-        <v>52918</v>
-      </c>
-      <c r="F59" s="15">
-        <v>78160</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C60" s="15">
+      <c r="C60" s="14">
         <v>29327</v>
       </c>
-      <c r="D60" s="15">
+      <c r="D60" s="14">
         <v>23923</v>
       </c>
-      <c r="E60" s="15">
+      <c r="E60" s="14">
         <v>24623</v>
       </c>
-      <c r="F60" s="15">
+      <c r="F60" s="14">
         <v>26300</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated with document changes from supervisor.
</commit_message>
<xml_diff>
--- a/TestHarness/Results/Results.xlsx
+++ b/TestHarness/Results/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ciaran\Workspace\MscDissertation\TestHarness\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A94A8D7-A75C-4D2A-9259-CD8627B1D809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD058CF-CCBB-4DC4-8B99-C244FBB4C650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{4D699BBE-F084-483C-BBD6-55F837A4A712}"/>
   </bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="53">
   <si>
     <t>SWARM_NUMBER</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>1,000,000 Particles</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -395,7 +398,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
@@ -414,8 +417,6 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
@@ -1466,6 +1467,87 @@
         <c:axId val="1466982832"/>
         <c:axId val="1466983248"/>
       </c:lineChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>TTSDTP</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="38100">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Summary!$M$32:$M$33</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Summary!$L$32:$L$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-94EF-4A8B-8F59-1F925EA36CFC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="552635391"/>
+        <c:axId val="267742287"/>
+      </c:scatterChart>
       <c:catAx>
         <c:axId val="1466982832"/>
         <c:scaling>
@@ -1572,6 +1654,61 @@
         <c:crossAx val="1466982832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="267742287"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:noFill/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="552635391"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="552635391"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="267742287"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -26973,10 +27110,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6321EF05-1508-47EE-9B24-FEEFC230091E}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:V35"/>
+  <dimension ref="A1:V44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4:V14"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28704,15 +28841,23 @@
       <c r="P31" s="4"/>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="L32" s="4"/>
-      <c r="M32" s="18"/>
+      <c r="L32" s="1">
+        <v>0</v>
+      </c>
+      <c r="M32" s="16">
+        <v>5</v>
+      </c>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
     </row>
     <row r="33" spans="12:16" x14ac:dyDescent="0.25">
-      <c r="L33" s="4"/>
-      <c r="M33" s="18"/>
+      <c r="L33" s="1">
+        <v>1</v>
+      </c>
+      <c r="M33" s="16">
+        <v>5</v>
+      </c>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
@@ -28730,6 +28875,11 @@
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
+    </row>
+    <row r="44" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L44" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28754,8 +28904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0233B6E-F38C-403B-A795-8C2A45CD94CE}">
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30082,15 +30232,8 @@
         <v>4385</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="16"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="17"/>
-    </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="16" t="s">
+      <c r="B53" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>